<commit_message>
v79: new category form
</commit_message>
<xml_diff>
--- a/Shopme Sample Users Data/Shopme Sample Users Data.xlsx
+++ b/Shopme Sample Users Data/Shopme Sample Users Data.xlsx
@@ -1574,7 +1574,7 @@
         <v>107</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="23.25">
       <c r="A23" s="6">
         <v>19</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>113</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="23.25">
       <c r="A24" s="6">
         <v>20</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>119</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="23.25">
       <c r="A25" s="6">
         <v>21</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>125</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="23.25">
       <c r="A26" s="6">
         <v>22</v>
       </c>
@@ -1678,7 +1678,7 @@
         <v>130</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="23.25">
       <c r="A27" s="6">
         <v>23</v>
       </c>

</xml_diff>